<commit_message>
Adicionado transformada de Hartley e modificada fourier
</commit_message>
<xml_diff>
--- a/docs/test/tempos.xlsx
+++ b/docs/test/tempos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>tempo</t>
   </si>
@@ -37,6 +37,9 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">107839 x10^006 </t>
   </si>
 </sst>
 </file>
@@ -381,13 +384,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -459,6 +465,14 @@
       </c>
       <c r="B9">
         <v>32768</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10">
+        <v>65536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>